<commit_message>
Endpoint de atualização de senha de usuário
</commit_message>
<xml_diff>
--- a/docs/orcamento.xlsx
+++ b/docs/orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desenvolvimento\Desktop\AgroTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C819CFB0-085D-4DCE-8CDF-D0D6E444ADF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E82E71E-8C5A-4111-A672-941FBE75B9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{211DDD06-3D26-4092-BDF8-45B9ACFDDFF6}"/>
   </bookViews>
@@ -328,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -391,6 +391,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -872,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFC5B09-AF59-4288-8FB1-3ED32641577E}">
   <dimension ref="B2:XFD34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,8 +1051,8 @@
       <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="19"/>
       <c r="F5" s="15"/>
       <c r="G5" s="19"/>

</xml_diff>